<commit_message>
i resolve one erro2
</commit_message>
<xml_diff>
--- a/Meuscodigosdomes8ao12/Exel manipulation/bdexcel.xlsx
+++ b/Meuscodigosdomes8ao12/Exel manipulation/bdexcel.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://senacspedu.sharepoint.com/sites/Section_sec_16379900278452/Documentos Compartilhados/General/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego.sgoncalves10\Documents\GitHub\repositoriodeestudosDatascience\Meuscodigosdomes8ao12\Exel manipulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{2E9707EE-BB1F-455E-9014-8003BC231DF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{727BB591-9AE0-43CC-89C5-50E7F601B89A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DDBEBD06-1FAD-4B6E-9621-840CFB590875}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F091E32A-000A-42EB-8759-3C5CD7E9824A}"/>
   </bookViews>
@@ -93,7 +93,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -492,7 +492,7 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
     <col min="2" max="2" width="24.140625" customWidth="1"/>
@@ -500,7 +500,7 @@
     <col min="4" max="4" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -514,7 +514,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -528,7 +528,7 @@
         <v>38362</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -542,7 +542,7 @@
         <v>38332</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -556,7 +556,7 @@
         <v>38885</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -570,7 +570,7 @@
         <v>39551</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -584,7 +584,7 @@
         <v>38132</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -598,7 +598,7 @@
         <v>39312</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -612,7 +612,7 @@
         <v>37685</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -626,7 +626,7 @@
         <v>38971</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -640,7 +640,7 @@
         <v>38668</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -661,15 +661,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101002D01605B63CFE04485B5EC762A3001C7" ma:contentTypeVersion="13" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="1204993477b1b293b674c6277874ebcc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d644159f-1f33-4448-adba-dadf15e1c1da" xmlns:ns3="1c315931-e46a-4c70-a5a3-aee59de18f03" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="97fdde551c2abda05e0111fd6c68215e" ns2:_="" ns3:_="">
     <xsd:import namespace="d644159f-1f33-4448-adba-dadf15e1c1da"/>
@@ -892,10 +883,58 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="d644159f-1f33-4448-adba-dadf15e1c1da"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1c315931-e46a-4c70-a5a3-aee59de18f03">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83DDBFF2-2B56-4DCA-BD64-F9D3A00C3FC1}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93B343EC-232D-4F85-9122-CDD1B869198E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="d644159f-1f33-4448-adba-dadf15e1c1da"/>
+    <ds:schemaRef ds:uri="1c315931-e46a-4c70-a5a3-aee59de18f03"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93B343EC-232D-4F85-9122-CDD1B869198E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83DDBFF2-2B56-4DCA-BD64-F9D3A00C3FC1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F791C82D-2F25-4F53-BAE1-58D65B95B3F6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>